<commit_message>
Newest updates to the git
</commit_message>
<xml_diff>
--- a/Hemolysis_Plots/20231207_Hemolysis_DIP_Polyplexes.xlsx
+++ b/Hemolysis_Plots/20231207_Hemolysis_DIP_Polyplexes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryellewright/Documents/Documents - Aryelle’s MacBook Air/Kumar-Biomaterials-Lab/Hemolysis_Plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688890EA-1C55-2745-BC44-79D49ACC7FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A863625-3210-3B45-A79C-0B0810DBDBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="660" windowWidth="21320" windowHeight="14100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="1640" windowWidth="21060" windowHeight="20600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate 1 - Sheet1" sheetId="1" r:id="rId1"/>
@@ -846,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:O41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40:I41"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1741,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B336AE3-3B61-6940-9F7C-EB9B49104A5F}">
   <dimension ref="C5:P33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2870,8 +2870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21881D3F-DDD3-8E4C-9937-294DB1CDBD74}">
   <dimension ref="C6:S33"/>
   <sheetViews>
-    <sheetView topLeftCell="G3" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7:M26"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6:S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4252,8 +4252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC10C112-2DF1-814B-81E8-A1E4708D59BA}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>